<commit_message>
doc updated - BASHA
</commit_message>
<xml_diff>
--- a/Documentation/RBLAnnualReportPackagesDetails.xlsx
+++ b/Documentation/RBLAnnualReportPackagesDetails.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12455"/>
+    <workbookView windowWidth="23040" windowHeight="9215"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Package ID</t>
   </si>
@@ -104,15 +104,6 @@
   </si>
   <si>
     <t>UNLIMITED</t>
-  </si>
-  <si>
-    <t>Extra User</t>
-  </si>
-  <si>
-    <t>Until Accounting Company Package Period</t>
-  </si>
-  <si>
-    <t>ADD-ON</t>
   </si>
 </sst>
 </file>
@@ -120,12 +111,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,35 +130,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -180,7 +142,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -188,6 +150,28 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -202,16 +186,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -225,6 +202,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -232,9 +232,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -250,44 +271,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -302,43 +286,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -350,109 +460,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -462,32 +470,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -511,14 +495,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -537,26 +525,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -580,6 +553,17 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -588,8 +572,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -608,166 +592,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -784,9 +757,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1134,13 +1104,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A8" sqref="$A8:$XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="18.5555555555556" customWidth="1"/>
     <col min="2" max="2" width="18.7777777777778" customWidth="1"/>
@@ -1323,7 +1293,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" ht="15.15" spans="1:9">
+    <row r="7" spans="1:9">
       <c r="A7" s="6">
         <v>600</v>
       </c>
@@ -1347,33 +1317,6 @@
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="6">
-        <v>700</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="6">
-        <v>1</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="6">
-        <v>300</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>